<commit_message>
update doc files, random benchmark results
</commit_message>
<xml_diff>
--- a/results/sixteen.local/ifl_talk/nf_bench.xlsx
+++ b/results/sixteen.local/ifl_talk/nf_bench.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sweirich/github/haskell/lambda-n-ways/results/sixteen.local/ifl_talk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66130E4E-8B47-1F48-9FEA-BC61A4F00611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F2BBF3-B51C-9447-9E89-096A530001A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="4220" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6976,7 +6976,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>